<commit_message>
last updated and pending for mapping
</commit_message>
<xml_diff>
--- a/docs/DB schemav0.1.xlsx
+++ b/docs/DB schemav0.1.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="94">
   <si>
     <t>Users</t>
   </si>
@@ -102,9 +102,6 @@
     <t>ph_id</t>
   </si>
   <si>
-    <t>project_status</t>
-  </si>
-  <si>
     <t>ph_phase</t>
   </si>
   <si>
@@ -183,9 +180,6 @@
     <t>s_created</t>
   </si>
   <si>
-    <t>project_details</t>
-  </si>
-  <si>
     <t>p_created</t>
   </si>
   <si>
@@ -295,6 +289,15 @@
   </si>
   <si>
     <t>s_deptid</t>
+  </si>
+  <si>
+    <t>0/1</t>
+  </si>
+  <si>
+    <t>projects</t>
+  </si>
+  <si>
+    <t>phase_status</t>
   </si>
 </sst>
 </file>
@@ -658,14 +661,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A52" sqref="A52"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="20.42578125" customWidth="1"/>
-    <col min="2" max="2" width="16.42578125" customWidth="1"/>
+    <col min="2" max="2" width="57.5703125" customWidth="1"/>
     <col min="3" max="3" width="53.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.7109375" customWidth="1"/>
   </cols>
@@ -687,7 +690,7 @@
         <v>11</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
@@ -700,7 +703,7 @@
         <v>12</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
@@ -713,7 +716,7 @@
         <v>12</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
@@ -726,7 +729,7 @@
         <v>12</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
@@ -739,7 +742,7 @@
         <v>12</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
@@ -768,7 +771,7 @@
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>15</v>
@@ -779,7 +782,7 @@
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>15</v>
@@ -790,7 +793,7 @@
     </row>
     <row r="12" spans="1:5" s="2" customFormat="1">
       <c r="A12" s="1" t="s">
-        <v>55</v>
+        <v>92</v>
       </c>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -805,7 +808,7 @@
         <v>11</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
@@ -818,7 +821,7 @@
         <v>12</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D14" s="4"/>
       <c r="E14" s="4"/>
@@ -831,7 +834,7 @@
         <v>12</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D15" s="4"/>
       <c r="E15" s="4"/>
@@ -844,7 +847,7 @@
         <v>12</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D16" s="4"/>
       <c r="E16" s="4"/>
@@ -857,7 +860,7 @@
         <v>12</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D17" s="4"/>
       <c r="E17" s="4"/>
@@ -870,7 +873,7 @@
         <v>12</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D18" s="4"/>
       <c r="E18" s="4"/>
@@ -883,43 +886,43 @@
         <v>12</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D19" s="4"/>
       <c r="E19" s="4"/>
     </row>
     <row r="20" spans="1:5" s="2" customFormat="1" ht="14.25" customHeight="1">
       <c r="A20" s="4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D20" s="4"/>
       <c r="E20" s="4"/>
     </row>
     <row r="21" spans="1:5" s="2" customFormat="1" ht="14.25" customHeight="1">
       <c r="A21" s="4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B21" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D21" s="4"/>
       <c r="E21" s="4"/>
     </row>
     <row r="22" spans="1:5" s="2" customFormat="1" ht="14.25" customHeight="1">
       <c r="A22" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C22" s="4"/>
       <c r="D22" s="4"/>
@@ -927,13 +930,13 @@
     </row>
     <row r="23" spans="1:5" s="2" customFormat="1" ht="14.25" customHeight="1">
       <c r="A23" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D23" s="4"/>
       <c r="E23" s="4"/>
@@ -947,7 +950,7 @@
     </row>
     <row r="25" spans="1:5" s="2" customFormat="1">
       <c r="A25" s="1" t="s">
-        <v>28</v>
+        <v>93</v>
       </c>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -956,13 +959,13 @@
     </row>
     <row r="26" spans="1:5" s="2" customFormat="1">
       <c r="A26" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D26" s="3">
         <v>1</v>
@@ -973,13 +976,13 @@
     </row>
     <row r="27" spans="1:5" s="2" customFormat="1">
       <c r="A27" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D27" s="3">
         <v>2</v>
@@ -990,13 +993,13 @@
     </row>
     <row r="28" spans="1:5" s="2" customFormat="1">
       <c r="A28" s="3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D28" s="3">
         <v>3</v>
@@ -1007,10 +1010,10 @@
     </row>
     <row r="29" spans="1:5" s="2" customFormat="1">
       <c r="A29" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C29" s="3"/>
       <c r="D29" s="3">
@@ -1048,30 +1051,30 @@
         <v>11</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D32" s="3"/>
       <c r="E32" s="3"/>
     </row>
     <row r="33" spans="1:5" s="2" customFormat="1">
       <c r="A33" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D33" s="3"/>
       <c r="E33" s="3"/>
     </row>
     <row r="34" spans="1:5" s="2" customFormat="1">
       <c r="A34" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C34" s="3"/>
       <c r="D34" s="3"/>
@@ -1086,7 +1089,7 @@
     </row>
     <row r="36" spans="1:5" s="2" customFormat="1">
       <c r="A36" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
@@ -1095,32 +1098,32 @@
     </row>
     <row r="37" spans="1:5" s="2" customFormat="1">
       <c r="A37" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B37" s="4"/>
       <c r="C37" s="4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D37" s="4"/>
       <c r="E37" s="4"/>
     </row>
     <row r="38" spans="1:5" s="2" customFormat="1">
       <c r="A38" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B38" s="4"/>
       <c r="C38" s="4" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D38" s="4"/>
       <c r="E38" s="4"/>
     </row>
     <row r="39" spans="1:5" s="2" customFormat="1">
       <c r="A39" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C39" s="4"/>
       <c r="D39" s="4"/>
@@ -1128,13 +1131,13 @@
     </row>
     <row r="40" spans="1:5" s="2" customFormat="1">
       <c r="A40" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D40" s="4"/>
       <c r="E40" s="4"/>
@@ -1148,7 +1151,7 @@
     </row>
     <row r="42" spans="1:5" s="2" customFormat="1">
       <c r="A42" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
@@ -1157,7 +1160,7 @@
     </row>
     <row r="43" spans="1:5" s="2" customFormat="1">
       <c r="A43" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B43"/>
       <c r="C43"/>
@@ -1166,7 +1169,7 @@
     </row>
     <row r="44" spans="1:5" s="2" customFormat="1">
       <c r="A44" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B44"/>
       <c r="C44"/>
@@ -1175,7 +1178,7 @@
     </row>
     <row r="45" spans="1:5" s="2" customFormat="1">
       <c r="A45" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B45"/>
       <c r="C45"/>
@@ -1191,7 +1194,7 @@
     </row>
     <row r="47" spans="1:5" s="2" customFormat="1">
       <c r="A47" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
@@ -1200,62 +1203,62 @@
     </row>
     <row r="48" spans="1:5" s="2" customFormat="1">
       <c r="A48" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B48" s="3"/>
       <c r="C48" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D48" s="3"/>
       <c r="E48" s="3"/>
     </row>
     <row r="49" spans="1:5" s="2" customFormat="1">
       <c r="A49" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B49" s="3"/>
       <c r="C49" s="3" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D49" s="3"/>
       <c r="E49" s="3"/>
     </row>
     <row r="50" spans="1:5" s="2" customFormat="1">
       <c r="A50" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B50" s="3"/>
       <c r="C50" s="3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D50" s="3"/>
       <c r="E50" s="3"/>
     </row>
     <row r="51" spans="1:5" s="2" customFormat="1">
       <c r="A51" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B51" s="3"/>
       <c r="C51" s="3" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D51" s="3"/>
       <c r="E51" s="3"/>
     </row>
     <row r="52" spans="1:5" s="2" customFormat="1">
       <c r="A52" s="3" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B52" s="3"/>
       <c r="C52" s="3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D52" s="3"/>
       <c r="E52" s="3"/>
     </row>
     <row r="53" spans="1:5" s="2" customFormat="1">
       <c r="A53" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B53" s="3"/>
       <c r="C53" s="3"/>
@@ -1271,7 +1274,7 @@
     </row>
     <row r="55" spans="1:5" s="2" customFormat="1">
       <c r="A55" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
@@ -1284,25 +1287,25 @@
       </c>
       <c r="B56" s="3"/>
       <c r="C56" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D56" s="3"/>
       <c r="E56" s="3"/>
     </row>
     <row r="57" spans="1:5" s="2" customFormat="1">
       <c r="A57" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B57" s="3"/>
       <c r="C57" s="3" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D57" s="3"/>
       <c r="E57" s="3"/>
     </row>
     <row r="58" spans="1:5" s="2" customFormat="1">
       <c r="A58" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B58" s="3"/>
       <c r="C58" s="3"/>
@@ -1318,7 +1321,7 @@
     </row>
     <row r="60" spans="1:5" s="2" customFormat="1">
       <c r="A60" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
@@ -1336,7 +1339,7 @@
     </row>
     <row r="62" spans="1:5" s="2" customFormat="1">
       <c r="A62" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B62" s="3"/>
       <c r="C62" s="3"/>
@@ -1345,9 +1348,11 @@
     </row>
     <row r="63" spans="1:5" s="2" customFormat="1">
       <c r="A63" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="B63" s="3"/>
+        <v>43</v>
+      </c>
+      <c r="B63" s="3" t="s">
+        <v>91</v>
+      </c>
       <c r="C63" s="3"/>
       <c r="D63" s="3"/>
       <c r="E63" s="3"/>

</xml_diff>